<commit_message>
changes done on 22
</commit_message>
<xml_diff>
--- a/Daily_update.xlsx
+++ b/Daily_update.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20403"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CAPRICON\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sai\Desktop\Git-Hub\New folder\dotnet_projectapi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68478864-25BC-474A-A5E4-07064DE289D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="5955" xr2:uid="{8176712B-7D87-4940-B70D-DCDB2355A787}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="5955"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>21-10-2023</t>
   </si>
@@ -61,12 +60,36 @@
   </si>
   <si>
     <t>5.Account created for diagram on Draw.io</t>
+  </si>
+  <si>
+    <t>22-10-2023</t>
+  </si>
+  <si>
+    <t>Docker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Dot_Net_Application</t>
+  </si>
+  <si>
+    <t>1.Download Docker</t>
+  </si>
+  <si>
+    <t>2.wsl2 required     wsl --install</t>
+  </si>
+  <si>
+    <t>3.enable Virulazation      bypressing f12</t>
+  </si>
+  <si>
+    <t>4.for checking taskmanager performance</t>
+  </si>
+  <si>
+    <t>5.window 21h1 not less than this</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -420,8 +443,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3085BFEF-D073-41AE-AD29-C88588065C59}">
-  <dimension ref="A1:D12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
@@ -497,6 +520,40 @@
         <v>11</v>
       </c>
     </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D1:D6"/>

</xml_diff>